<commit_message>
Now it's available to save a entire excel with Student and Parent. Also, the error are written on the sheet
</commit_message>
<xml_diff>
--- a/Estudiantes.xlsx
+++ b/Estudiantes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>Nombre</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>1156968958</t>
+  </si>
+  <si>
+    <t>[[400] during [POST] to [http://localhost:8090/click-escuela/school-admin/school/1234/student] [StudentController#createStudent(String,StudentApi)]: [Ya existe el estudiante]]</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>98632585</t>
+  </si>
+  <si>
+    <t>[[400] during [POST] to [http://localhost:8090/click-escuela/school-admin/school/1234/student] [StudentController#createStudent(String,StudentApi)]: [{"status":400,"message":"validation error","validationErrors":[{"message":"Locality cannot be null","field":"parentApi.adressApi.locality"},{"message":"CellPhone cannot be null","field":"parentApi.cel... (1882 bytes)]]</t>
   </si>
 </sst>
 </file>
@@ -176,12 +188,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE62718"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -196,19 +220,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE62718"/>
+      <color rgb="FF9F1B11"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -497,91 +534,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T1000"/>
+  <dimension ref="A1:AMD999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
-    <col min="12" max="1018" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="20" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="22" max="1018" width="14.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="U1" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" customHeight="1">
+    <row r="2" spans="1:21" ht="165.75">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -642,8 +684,11 @@
       <c r="T2" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="U2" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" ht="15.75" customHeight="1">
+    <row r="3" spans="1:21" ht="165.75">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -704,22 +749,52 @@
       <c r="T3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="U3" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="5" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="6" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="9" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:20" ht="15.75" customHeight="1">
-      <c r="R12" s="5"/>
+    <row r="4" spans="1:21" ht="331.5">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:20" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:20" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:21" ht="15.75" customHeight="1">
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:21" ht="15.75" customHeight="1">
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:21" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1703,15 +1778,15 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>
     <hyperlink ref="T2" r:id="rId3"/>
     <hyperlink ref="T3" r:id="rId4"/>
+    <hyperlink ref="G4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creating test for StudentBulkUpload
</commit_message>
<xml_diff>
--- a/Estudiantes.xlsx
+++ b/Estudiantes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>Nombre</t>
   </si>
@@ -150,22 +150,16 @@
     <t>1156968958</t>
   </si>
   <si>
-    <t>[[400] during [POST] to [http://localhost:8090/click-escuela/school-admin/school/1234/student] [StudentController#createStudent(String,StudentApi)]: [Ya existe el estudiante]]</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
     <t>98632585</t>
   </si>
   <si>
-    <t>[[400] during [POST] to [http://localhost:8090/click-escuela/school-admin/school/1234/student] [StudentController#createStudent(String,StudentApi)]: [{"status":400,"message":"validation error","validationErrors":[{"message":"Locality cannot be null","field":"parentApi.adressApi.locality"},{"message":"CellPhone cannot be null","field":"parentApi.cel... (1882 bytes)]]</t>
-  </si>
-  <si>
-    <t>[ Ya existe el estudiante]</t>
-  </si>
-  <si>
-    <t>[ {"status"]</t>
+    <t>[[400] during [POST] to [http://school-admin/school/1234/student] [StudentController#createStudent(String,StudentApi)]: [Ya existe el estudiante]]</t>
+  </si>
+  <si>
+    <t>[[400] during [POST] to [http://school-admin/school/1234/student] [StudentController#createStudent(String,StudentApi)]: [{"status":400,"message":"validation error","validationErrors":[{"message":"Grade cannot be null","field":"grade"},{"message":"Street cannot be null","field":"adressApi.street"},{"message":"Name cannot... (1882 bytes)]]</t>
   </si>
 </sst>
 </file>
@@ -541,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U999"/>
+  <dimension ref="A1:V999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -565,7 +559,7 @@
     <col min="22" max="1018" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -627,10 +621,10 @@
         <v>6</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="165.75">
+    <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -691,11 +685,11 @@
       <c r="T2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="6" t="s">
-        <v>43</v>
+      <c r="U2" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="165.75">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -756,11 +750,11 @@
       <c r="T3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="6" t="s">
-        <v>43</v>
+      <c r="U3" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="331.5">
+    <row r="4" spans="1:22">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -768,7 +762,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -782,46 +776,46 @@
       <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="U4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1">
+    <row r="5" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:22" ht="15.75" customHeight="1">
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1">
+    <row r="9" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1">
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="U21" t="s">
-        <v>48</v>
-      </c>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1">
+      <c r="V16" s="5"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="17" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="18" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="19" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="20" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="21" spans="21:21" ht="15.75" customHeight="1">
+      <c r="U21"/>
+    </row>
+    <row r="22" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="23" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="24" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="25" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="26" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="27" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="28" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="29" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="30" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="31" spans="21:21" ht="15.75" customHeight="1"/>
+    <row r="32" spans="21:21" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>